<commit_message>
Fixed bug in Model_patients using wrong data to test model
</commit_message>
<xml_diff>
--- a/PrecisionRecall.xlsx
+++ b/PrecisionRecall.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Precision</t>
   </si>
@@ -60,13 +60,16 @@
   </si>
   <si>
     <t>Walk</t>
+  </si>
+  <si>
+    <t>MEAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -76,6 +79,23 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -113,6 +133,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,33 +419,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="1"/>
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -438,26 +465,32 @@
       <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="O2" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -476,26 +509,34 @@
       <c r="F3" s="4">
         <v>0.84606907157990896</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="8">
+        <f>AVERAGE(B3:F3)</f>
+        <v>0.51874948639003615</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>0.76397507064976899</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>2.5540556334735901E-2</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="5">
         <v>0.51458987593385797</v>
       </c>
-      <c r="L3" s="4">
+      <c r="M3" s="4">
         <v>0.650410961379014</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>0.34445501889248997</v>
       </c>
+      <c r="O3" s="8">
+        <f>AVERAGE(J3:N3)</f>
+        <v>0.45979429663797333</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -514,26 +555,34 @@
       <c r="F4" s="4">
         <v>0.84718706012269096</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="8">
+        <f t="shared" ref="G4:G6" si="0">AVERAGE(B4:F4)</f>
+        <v>0.59982500142377937</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="6">
         <v>0.83730005347551195</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>2.4612021857923501E-2</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>3.9007432270438798E-2</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>0.79240677441257301</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>0.89125233606120002</v>
       </c>
+      <c r="O4" s="8">
+        <f t="shared" ref="O4:O5" si="1">AVERAGE(J4:N4)</f>
+        <v>0.51691572361552951</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -552,26 +601,34 @@
       <c r="F5" s="5">
         <v>0.90745562629371701</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.6630433018297397</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>0.727612734939592</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>0.117824962290614</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="6">
         <v>0.44985186600363403</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <v>0.75729780887325504</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>0.88758194027666804</v>
       </c>
+      <c r="O5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.5880338624767526</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -590,32 +647,40 @@
       <c r="F6" s="4">
         <v>0.89734479841018699</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>0.70701681229753444</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="5">
         <v>0.87197726757541805</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>0.330462934149234</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>0.43845506485192898</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>0.79553015070642896</v>
       </c>
-      <c r="M6" s="5">
+      <c r="N6" s="5">
         <v>0.91143024866048805</v>
+      </c>
+      <c r="O6" s="10">
+        <f>AVERAGE(J6:N6)</f>
+        <v>0.66957113318869954</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="I1:N1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:F6">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="B3:G6">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -628,7 +693,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:M6">
+  <conditionalFormatting sqref="J3:N6">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6F8D7DA3-8373-4717-97DC-91768484B015}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O6">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -637,7 +716,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6F8D7DA3-8373-4717-97DC-91768484B015}</x14:id>
+          <x14:id>{CAD10A5C-1CE1-4A38-82BE-28DE6CC56B5C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -656,7 +735,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B3:F6</xm:sqref>
+          <xm:sqref>B3:G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6F8D7DA3-8373-4717-97DC-91768484B015}">
@@ -667,7 +746,18 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I3:M6</xm:sqref>
+          <xm:sqref>J3:N6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CAD10A5C-1CE1-4A38-82BE-28DE6CC56B5C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O3:O6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>